<commit_message>
reverse RT recursive and matching layers losses for flat and wedge
</commit_message>
<xml_diff>
--- a/Phase_distribution_60.xlsx
+++ b/Phase_distribution_60.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,730 +440,850 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>-495.3132398834571</v>
+        <v>-0.5177348774463787</v>
       </c>
       <c r="B2" t="n">
-        <v>-657.6116726519258</v>
+        <v>-482.8672876447307</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>-463.9505539648974</v>
+        <v>-0.5078098721269414</v>
       </c>
       <c r="B3" t="n">
-        <v>-650.4044700190886</v>
+        <v>-481.6889470267456</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>-435.7493141243253</v>
+        <v>-0.4978848667350946</v>
       </c>
       <c r="B4" t="n">
-        <v>-644.000430903455</v>
+        <v>-480.5106064001636</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>-410.0150763420276</v>
+        <v>-0.4879598613794522</v>
       </c>
       <c r="B5" t="n">
-        <v>-638.2212978802244</v>
+        <v>-479.3322657778801</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>-386.2562410859509</v>
+        <v>-0.4780348560592672</v>
       </c>
       <c r="B6" t="n">
-        <v>-632.9412338109012</v>
+        <v>-478.1539251598061</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>-364.1132727749131</v>
+        <v>-0.4681098506681684</v>
       </c>
       <c r="B7" t="n">
-        <v>-628.0684179789262</v>
+        <v>-476.9755845333129</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>-343.3159766611511</v>
+        <v>-0.4581848453125258</v>
       </c>
       <c r="B8" t="n">
-        <v>-623.5339752266767</v>
+        <v>-475.7972439110295</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>-323.6563553483092</v>
+        <v>-0.4482598399568842</v>
       </c>
       <c r="B9" t="n">
-        <v>-619.2849732743547</v>
+        <v>-474.6189032887459</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>-304.9712167003029</v>
+        <v>-0.4383348346356992</v>
       </c>
       <c r="B10" t="n">
-        <v>-615.2799349988315</v>
+        <v>-473.4405626705533</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>-287.1302841159158</v>
+        <v>-0.4284098292203118</v>
       </c>
       <c r="B11" t="n">
-        <v>-611.4857840284346</v>
+        <v>-472.2622220411765</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>-270.0279271356117</v>
+        <v>-0.4184848239239157</v>
       </c>
       <c r="B12" t="n">
-        <v>-607.8757268632309</v>
+        <v>-471.0838814259268</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>-253.5773604357529</v>
+        <v>-0.4085598185343151</v>
       </c>
       <c r="B13" t="n">
-        <v>-604.4277675811018</v>
+        <v>-469.9055407996117</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>-237.706497403797</v>
+        <v>-0.3986348132121328</v>
       </c>
       <c r="B14" t="n">
-        <v>-601.123645309596</v>
+        <v>-468.7272001813007</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>-222.3547351188077</v>
+        <v>-0.3887098078230316</v>
       </c>
       <c r="B15" t="n">
-        <v>-597.9480189267263</v>
+        <v>-467.5488595550447</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>-207.4705981212492</v>
+        <v>-0.378784802443225</v>
       </c>
       <c r="B16" t="n">
-        <v>-594.887868396679</v>
+        <v>-466.3705189298922</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>-193.010147803322</v>
+        <v>-0.3688597971117475</v>
       </c>
       <c r="B17" t="n">
-        <v>-591.9320811644819</v>
+        <v>-465.1921783104776</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>-178.9353697818079</v>
+        <v>-0.358934791764849</v>
       </c>
       <c r="B18" t="n">
-        <v>-589.0710541329734</v>
+        <v>-464.0138376892321</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>-165.2132846276789</v>
+        <v>-0.3490097864004638</v>
       </c>
       <c r="B19" t="n">
-        <v>-586.2964591325651</v>
+        <v>-462.8354970659106</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>-151.8150467946928</v>
+        <v>-0.3390847810448211</v>
       </c>
       <c r="B20" t="n">
-        <v>-583.6010169766611</v>
+        <v>-461.6571564436269</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>-138.7152176255904</v>
+        <v>-0.3291597757208907</v>
       </c>
       <c r="B21" t="n">
-        <v>-580.9783159754797</v>
+        <v>-460.4788158251083</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>-125.8913029647672</v>
+        <v>-0.3192347703335372</v>
       </c>
       <c r="B22" t="n">
-        <v>-578.422690596056</v>
+        <v>-459.3004751990599</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>-113.3232959014369</v>
+        <v>-0.3093097650091061</v>
       </c>
       <c r="B23" t="n">
-        <v>-575.9291063796618</v>
+        <v>-458.1221345804819</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>-100.9933241467511</v>
+        <v>-0.2993847596532149</v>
       </c>
       <c r="B24" t="n">
-        <v>-573.4930700981612</v>
+        <v>-456.9437939581687</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>-88.88528117350343</v>
+        <v>-0.2894597542444678</v>
       </c>
       <c r="B25" t="n">
-        <v>-571.1105402955457</v>
+        <v>-455.7654533295803</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>-76.98469185246165</v>
+        <v>-0.2795347489414319</v>
       </c>
       <c r="B26" t="n">
-        <v>-568.7778869414727</v>
+        <v>-454.5871127135425</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>-65.27842139053173</v>
+        <v>-0.2696097435855395</v>
       </c>
       <c r="B27" t="n">
-        <v>-566.4918223932376</v>
+        <v>-453.4087720912291</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>-53.75452517249462</v>
+        <v>-0.2596847381996842</v>
       </c>
       <c r="B28" t="n">
-        <v>-564.2493620345416</v>
+        <v>-452.2304314653586</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>-42.4021424052842</v>
+        <v>-0.2497597328440431</v>
       </c>
       <c r="B29" t="n">
-        <v>-562.0477948827538</v>
+        <v>-451.0520908430752</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>-31.21134835579261</v>
+        <v>-0.2398347275178642</v>
       </c>
       <c r="B30" t="n">
-        <v>-559.8846473733422</v>
+        <v>-449.8737502242897</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>-20.17301093978746</v>
+        <v>-0.229909722132759</v>
       </c>
       <c r="B31" t="n">
-        <v>-557.7576491785692</v>
+        <v>-448.6954095985081</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>-9.27877022182509</v>
+        <v>-0.2199847167771163</v>
       </c>
       <c r="B32" t="n">
-        <v>-555.6647236565558</v>
+        <v>-447.5170689762245</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>1.479142643763372</v>
+        <v>-0.2100597114214736</v>
       </c>
       <c r="B33" t="n">
-        <v>-553.6039481245386</v>
+        <v>-446.3387283539408</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>12.10785452187448</v>
+        <v>-0.2001347060942971</v>
       </c>
       <c r="B34" t="n">
-        <v>-551.5735593744988</v>
+        <v>-445.1603877350369</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>22.61397574269618</v>
+        <v>-0.1902097007384047</v>
       </c>
       <c r="B35" t="n">
-        <v>-549.5719258226146</v>
+        <v>-443.9820471127236</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>33.00366278654908</v>
+        <v>-0.180284695382514</v>
       </c>
       <c r="B36" t="n">
-        <v>-547.5975322590366</v>
+        <v>-442.8037064904105</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>43.2826143221718</v>
+        <v>-0.1703596900266216</v>
       </c>
       <c r="B37" t="n">
-        <v>-545.6489776562943</v>
+        <v>-441.6253658680974</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>53.45614571169123</v>
+        <v>-0.1604346846432633</v>
       </c>
       <c r="B38" t="n">
-        <v>-543.7249583758334</v>
+        <v>-440.4470252425232</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>63.52923215724812</v>
+        <v>-0.1505096793148384</v>
       </c>
       <c r="B39" t="n">
-        <v>-541.8242576886141</v>
+        <v>-439.2686846234709</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>73.50648728641195</v>
+        <v>-0.140584673958946</v>
       </c>
       <c r="B40" t="n">
-        <v>-539.9457477237057</v>
+        <v>-438.0903440011577</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>83.39230244083805</v>
+        <v>-0.1306596686030553</v>
       </c>
       <c r="B41" t="n">
-        <v>-538.0883613622433</v>
+        <v>-436.9120033788447</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>93.19072180356076</v>
+        <v>-0.1207346632206957</v>
       </c>
       <c r="B42" t="n">
-        <v>-536.2511140763772</v>
+        <v>-435.7336627533891</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>102.9055612015979</v>
+        <v>-0.1108096578650527</v>
       </c>
       <c r="B43" t="n">
-        <v>-534.4330800524965</v>
+        <v>-434.5553221311055</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>112.5404351216524</v>
+        <v>-0.1008846525094117</v>
       </c>
       <c r="B44" t="n">
-        <v>-532.6333858174294</v>
+        <v>-433.3769815088221</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>122.0986990148276</v>
+        <v>-0.09095964717948724</v>
       </c>
       <c r="B45" t="n">
-        <v>-530.8512197946244</v>
+        <v>-432.1986408895918</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>131.5835769638648</v>
+        <v>-0.08103464180617249</v>
       </c>
       <c r="B46" t="n">
-        <v>-529.0858073625169</v>
+        <v>-431.0203002652101</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>140.9980653872597</v>
+        <v>-0.07110963642528623</v>
       </c>
       <c r="B47" t="n">
-        <v>-527.3364278181689</v>
+        <v>-429.8419596399294</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>150.3449706535316</v>
+        <v>-0.06118463108684238</v>
       </c>
       <c r="B48" t="n">
-        <v>-525.602406408487</v>
+        <v>-428.6636190196878</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>159.6270118488362</v>
+        <v>-0.05125962575592068</v>
       </c>
       <c r="B49" t="n">
-        <v>-523.8830944388442</v>
+        <v>-427.4852784003392</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>168.8467099440935</v>
+        <v>-0.04133462040002839</v>
       </c>
       <c r="B50" t="n">
-        <v>-522.1778890882249</v>
+        <v>-426.3069377780259</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>178.0064855337172</v>
+        <v>-0.03140961504413733</v>
       </c>
       <c r="B51" t="n">
-        <v>-520.4862145989754</v>
+        <v>-425.1285971557128</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>187.1085940439045</v>
+        <v>-0.02148460968824496</v>
       </c>
       <c r="B52" t="n">
-        <v>-518.8075336248504</v>
+        <v>-423.9502565333996</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>196.155209765035</v>
+        <v>-0.0115596043086321</v>
       </c>
       <c r="B53" t="n">
-        <v>-517.1413311300827</v>
+        <v>-422.77191590827</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>205.1483787848113</v>
+        <v>-0.001634598976461639</v>
       </c>
       <c r="B54" t="n">
-        <v>-515.4871225501918</v>
+        <v>-421.5935752887731</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>214.090051765371</v>
+        <v>0.008290406387131301</v>
       </c>
       <c r="B55" t="n">
-        <v>-513.8444472602985</v>
+        <v>-420.4152346655457</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>222.9820770264741</v>
+        <v>0.01821541173532145</v>
       </c>
       <c r="B56" t="n">
-        <v>-512.2128693998401</v>
+        <v>-419.2368940441469</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>231.8262231689834</v>
+        <v>0.02814041709121383</v>
       </c>
       <c r="B57" t="n">
-        <v>-510.5919733060387</v>
+        <v>-418.0585534218336</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>240.6241655646026</v>
+        <v>0.03806542246957818</v>
       </c>
       <c r="B58" t="n">
-        <v>-508.9813656135118</v>
+        <v>-416.8802127968524</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>249.3774993472771</v>
+        <v>0.0479904278029971</v>
       </c>
       <c r="B59" t="n">
-        <v>-507.3806725174708</v>
+        <v>-415.7018721772073</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>258.0877700219445</v>
+        <v>0.05791543315888949</v>
       </c>
       <c r="B60" t="n">
-        <v>-505.7895338582389</v>
+        <v>-414.5235315548941</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>266.7563924113195</v>
+        <v>0.06784043850072774</v>
       </c>
       <c r="B61" t="n">
-        <v>-504.2076176265212</v>
+        <v>-413.3451909342493</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>275.3847680867908</v>
+        <v>0.07776544389214612</v>
       </c>
       <c r="B62" t="n">
-        <v>-502.6345982312205</v>
+        <v>-412.1668503077183</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>283.9742100097687</v>
+        <v>0.08769044924016869</v>
       </c>
       <c r="B63" t="n">
-        <v>-501.070170007332</v>
+        <v>-410.9885096863394</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>292.5260014253171</v>
+        <v>0.0976154546034298</v>
       </c>
       <c r="B64" t="n">
-        <v>-499.5140362418041</v>
+        <v>-409.8101690631513</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>301.0413407330738</v>
+        <v>0.1075404599449252</v>
       </c>
       <c r="B65" t="n">
-        <v>-497.9659189931137</v>
+        <v>-408.6318284425473</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>309.5213831852338</v>
+        <v>0.1174654652942393</v>
       </c>
       <c r="B66" t="n">
-        <v>-496.4255512898129</v>
+        <v>-407.453487821015</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>317.9672358783133</v>
+        <v>0.1273904706640041</v>
       </c>
       <c r="B67" t="n">
-        <v>-494.8926778543966</v>
+        <v>-406.2751471970547</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>326.3799574605766</v>
+        <v>0.137315476032239</v>
       </c>
       <c r="B68" t="n">
-        <v>-493.3670549785164</v>
+        <v>-405.0968065732761</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>334.7605643638912</v>
+        <v>0.1472404813816405</v>
       </c>
       <c r="B69" t="n">
-        <v>-491.8484492264165</v>
+        <v>-403.9184659517335</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>343.1099983142942</v>
+        <v>0.1571654867312679</v>
       </c>
       <c r="B70" t="n">
-        <v>-490.3366431616561</v>
+        <v>-402.740125330164</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>351.4292177318595</v>
+        <v>0.1670904920929241</v>
       </c>
       <c r="B71" t="n">
-        <v>-488.8314186493271</v>
+        <v>-401.5617847071665</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>359.7191165375762</v>
+        <v>0.1770154974427763</v>
       </c>
       <c r="B72" t="n">
-        <v>-487.332571432865</v>
+        <v>-400.3834440855703</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>367.9805195018171</v>
+        <v>0.1869405027985312</v>
       </c>
       <c r="B73" t="n">
-        <v>-485.8399118301787</v>
+        <v>-399.2051034632734</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>376.2142763904725</v>
+        <v>0.196865508154285</v>
       </c>
       <c r="B74" t="n">
-        <v>-484.3532476023225</v>
+        <v>-398.0267628409767</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>384.4211694642041</v>
+        <v>0.20679051351004</v>
       </c>
       <c r="B75" t="n">
-        <v>-482.8724005637036</v>
+        <v>-396.8484222186797</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>392.6019405677135</v>
+        <v>0.2167155188711345</v>
       </c>
       <c r="B76" t="n">
-        <v>-481.397201574335</v>
+        <v>-395.6700815957488</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>400.7573232250001</v>
+        <v>0.2266405242215485</v>
       </c>
       <c r="B77" t="n">
-        <v>-479.9274846554209</v>
+        <v>-394.491740974086</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>408.8880245306248</v>
+        <v>0.2365655295773036</v>
       </c>
       <c r="B78" t="n">
-        <v>-478.463090170459</v>
+        <v>-393.313400351789</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>416.9946978283286</v>
+        <v>0.2464905349330572</v>
       </c>
       <c r="B79" t="n">
-        <v>-477.0038696568513</v>
+        <v>-392.1350597294922</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>425.0780089187184</v>
+        <v>0.2564155402888121</v>
       </c>
       <c r="B80" t="n">
-        <v>-475.5496738243022</v>
+        <v>-390.9567191071953</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>433.1385609217829</v>
+        <v>0.2663405456278367</v>
       </c>
       <c r="B81" t="n">
-        <v>-474.1003660045704</v>
+        <v>-389.7783784868847</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>441.1769573817579</v>
+        <v>0.2762655510003207</v>
       </c>
       <c r="B82" t="n">
-        <v>-472.6558107244414</v>
+        <v>-388.6000378626015</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>449.1937749413499</v>
+        <v>0.2861905563398462</v>
       </c>
       <c r="B83" t="n">
-        <v>-471.2158785571273</v>
+        <v>-387.4216972422315</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>457.1895671695858</v>
+        <v>0.2961155617002915</v>
       </c>
       <c r="B84" t="n">
-        <v>-469.7804453701335</v>
+        <v>-386.2433566193777</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>465.1648656383367</v>
+        <v>0.3060405670675844</v>
       </c>
       <c r="B85" t="n">
-        <v>-468.3493920720859</v>
+        <v>-385.0650159957109</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>473.120184310558</v>
+        <v>0.3159655724233379</v>
       </c>
       <c r="B86" t="n">
-        <v>-466.9226037693633</v>
+        <v>-383.8866753734142</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>481.056014528922</v>
+        <v>0.3258905777638621</v>
       </c>
       <c r="B87" t="n">
-        <v>-465.4999706124206</v>
+        <v>-382.7083347529255</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>488.9728411060948</v>
+        <v>0.3358155831388407</v>
       </c>
       <c r="B88" t="n">
-        <v>-464.0813848620039</v>
+        <v>-381.5299941283462</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>496.8711264083544</v>
+        <v>0.3457405884906016</v>
       </c>
       <c r="B89" t="n">
-        <v>-462.6667436968606</v>
+        <v>-380.3516535065235</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>504.7513035734607</v>
+        <v>0.3556655938356427</v>
       </c>
       <c r="B90" t="n">
-        <v>-461.2559503812225</v>
+        <v>-379.1733128854985</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>512.6138096191434</v>
+        <v>0.3655905991878796</v>
       </c>
       <c r="B91" t="n">
-        <v>-459.8489082944338</v>
+        <v>-377.9949722636192</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>520.4590549474675</v>
+        <v>0.3755156045578651</v>
       </c>
       <c r="B92" t="n">
-        <v>-458.4455263526936</v>
+        <v>-376.8166316396328</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>0.3854406098998875</v>
+      </c>
+      <c r="B93" t="n">
+        <v>-375.6382910189662</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>0.3953656152558907</v>
+      </c>
+      <c r="B94" t="n">
+        <v>-374.4599503966398</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>0.4052906206118955</v>
+      </c>
+      <c r="B95" t="n">
+        <v>-373.2816097743132</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>0.415215625970994</v>
+      </c>
+      <c r="B96" t="n">
+        <v>-372.1032691516193</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>0.425140631326885</v>
+      </c>
+      <c r="B97" t="n">
+        <v>-370.9249285293062</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>0.4350656366770391</v>
+      </c>
+      <c r="B98" t="n">
+        <v>-369.7465879076742</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>0.4449906420331547</v>
+      </c>
+      <c r="B99" t="n">
+        <v>-368.5682472853345</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>0.4549156473945606</v>
+      </c>
+      <c r="B100" t="n">
+        <v>-367.3899066623666</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>0.4648406527555168</v>
+      </c>
+      <c r="B101" t="n">
+        <v>-366.2115660394521</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>0.4747656581111831</v>
+      </c>
+      <c r="B102" t="n">
+        <v>-365.0332254171658</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>0.4846906634668506</v>
+      </c>
+      <c r="B103" t="n">
+        <v>-363.8548847948791</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>0.4946156688181271</v>
+      </c>
+      <c r="B104" t="n">
+        <v>-362.6765441731139</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>0.504540674188921</v>
+      </c>
+      <c r="B105" t="n">
+        <v>-361.4982035490315</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>0.514465679544339</v>
+      </c>
+      <c r="B106" t="n">
+        <v>-360.3198629267746</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>0.5243906848997554</v>
+      </c>
+      <c r="B107" t="n">
+        <v>-359.1415223045179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>